<commit_message>
adding Kody's CSS to to the final code and making some tab js changes and changed the look of the whole page
</commit_message>
<xml_diff>
--- a/FinalProject/docs/Task_assignment.xlsx
+++ b/FinalProject/docs/Task_assignment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwspedu-my.sharepoint.com/personal/imobe456_uwsp_edu/Documents/Documents/CNMT 310/FinalProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwspedu-my.sharepoint.com/personal/imobe456_uwsp_edu/Documents/Documents/CNMT 310/FinalProject/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB49B5EB-81E5-4CBD-81C4-3DBA17DDDCCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{FB49B5EB-81E5-4CBD-81C4-3DBA17DDDCCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64575F09-82F7-4E99-BA98-95E17DD1B425}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{23A0825C-E0AC-4A34-9541-57F8F04D4D6A}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{23A0825C-E0AC-4A34-9541-57F8F04D4D6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
-  <si>
-    <t>SPRING ONE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t xml:space="preserve">Isaac </t>
   </si>
   <si>
-    <t>Cody</t>
-  </si>
-  <si>
     <t>Nick</t>
   </si>
   <si>
@@ -63,6 +57,48 @@
   </si>
   <si>
     <t>WireFrame Bookmarks Page</t>
+  </si>
+  <si>
+    <t>SPRINT ONE</t>
+  </si>
+  <si>
+    <t>SPRINT TWO</t>
+  </si>
+  <si>
+    <t>Isaac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Functionality </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Handling </t>
+  </si>
+  <si>
+    <t>Automated Testing</t>
+  </si>
+  <si>
+    <t>Testing/Test Plan</t>
+  </si>
+  <si>
+    <t>Error Handling/Javascript Functionality</t>
+  </si>
+  <si>
+    <t>SPRINT THREE</t>
+  </si>
+  <si>
+    <t>Kody</t>
+  </si>
+  <si>
+    <t>Autocomplete Functionality</t>
+  </si>
+  <si>
+    <t>CSS/Clean look</t>
+  </si>
+  <si>
+    <t>CSS/Clean Look</t>
+  </si>
+  <si>
+    <t>Add Visit AJAX</t>
   </si>
 </sst>
 </file>
@@ -414,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CEB5D36-6972-4958-AF7F-08D0F213E198}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,49 +466,134 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>